<commit_message>
Fix DeleteRow and DeleteColumn Tests involving deleting entire charts / data validation source ranges / etc.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/ComboFromExcel.xlsx
+++ b/EPPlusTest/Workbooks/ComboFromExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cgypt\Desktop\test cases\charts for regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Source\Repos\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" concurrentManualCount="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -195,70 +195,70 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>100</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>77</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>47</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>85</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -317,73 +317,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>75</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>78</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>97</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>97</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>79</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,73 +458,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>97</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>77</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>88</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>53</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>57</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>75</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>26</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -590,6 +590,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="797348592"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -647,6 +648,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="797339736"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1293,16 +1295,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>271462</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>576262</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1589,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B19:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,259 +1614,259 @@
       </c>
       <c r="C20">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="D20">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C21">
         <f t="shared" ref="B21:D42" ca="1" si="0">RANDBETWEEN(10,100)</f>
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
@@ -1874,57 +1876,57 @@
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>